<commit_message>
Edits to BRP and Research Emphasis updates
</commit_message>
<xml_diff>
--- a/brp/tcrb/documents/SCTC_Products.xlsx
+++ b/brp/tcrb/documents/SCTC_Products.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\websites\dccpsweb\brp\tcrb\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="6U4tIHNbv4mY6xOcx87vVPnRcvpp7W7d8eDrjvb2PoWSkRgSk6HQpkBP5k4Tiymb6YPRMjybDEYGKYl/FQUHdQ==" workbookSaltValue="6G4t7U7wHVs+30cMMFxVoA==" workbookSpinCount="100000" lockStructure="1"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="mw6HHvNszZvrK+1oflgNxWY18XPwBaS5+aauZtUexKMXow6FxzuSTo0B3S27pAkZa+69KHGL/g2D9WwOHIc0Wg==" workbookSaltValue="K+vZPm8ZdwiGv+Frzc5+sA==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Other Products" sheetId="3" r:id="rId1"/>
@@ -2286,7 +2286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -2703,6 +2703,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="pH4xnTywwsQszctAClj95P5cXett+RDOCFDNcCgxreLCmF+nW8EXTTqvPuOtg1NsEtRGhHkudaGGto1x9cAxUA==" saltValue="EZbEwkPeXGoyCu6k1zB6eg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <hyperlinks>
     <hyperlink ref="E9" r:id="rId1"/>
     <hyperlink ref="E8" r:id="rId2"/>
@@ -2733,7 +2734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB417"/>
   <sheetViews>
-    <sheetView topLeftCell="A400" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A400" workbookViewId="0">
       <selection activeCell="B426" sqref="B426"/>
     </sheetView>
   </sheetViews>
@@ -12164,6 +12165,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="3kelYpZEu6HHImVpegC87+9iFCL5ERoBSh74n5qAbWKbh27f9TwyBhqVCVrTrbw1PUgYwVJWYVfHZCWp3TOOmQ==" saltValue="yDKFgXzI60t4gB1aUahQQw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <sortState ref="A24:AB98">
     <sortCondition ref="D24:D98"/>
     <sortCondition ref="B24:B98"/>

</xml_diff>